<commit_message>
add cited, year tabs
- add Cited by tabs
- add year tabs
</commit_message>
<xml_diff>
--- a/gsc1-20.xlsx
+++ b/gsc1-20.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20371"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SIMHYUNCHAE\Documents\GitHub\meta_bcblpap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BCBL2\Documents\GitHub\meta_bcblpap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD2CD07-417B-463D-8F4E-4319D6CEB654}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BA97AD-38A0-4252-AEE2-684FF128D956}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>Title</t>
   </si>
@@ -31,185 +31,205 @@
     <t>Journal</t>
   </si>
   <si>
+    <t>Cited By</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
     <t>Inhibitory effects of aloin on TGFBIp-mediated septic responses</t>
   </si>
   <si>
+    <t>Biapenem reduces sepsis mortality via barrier protective pathways against HMGB1-mediated septic responses</t>
+  </si>
+  <si>
+    <t>Selective inhibitory effects of HYIpro-3-1 on CYP1A2 in human liver microsomes.</t>
+  </si>
+  <si>
+    <t>Impacts of Drug Interactions on Pharmacokinetics and the Brain Transporters: A Recent Review of Natural Compound-Drug Interactions in Brain Disorders</t>
+  </si>
+  <si>
+    <t>Barrier protective functions of hederacolchiside-E against HMGB1-mediated septic responses</t>
+  </si>
+  <si>
+    <t>Natural Antioxidant and Anti-Inflammatory Compounds in Foodstuff or Medicinal Herbs Inducing Heme Oxygenase-1 Expression</t>
+  </si>
+  <si>
+    <t>Tie2-mediated vascular remodeling by ferritin-based protein C nanoparticles confers antitumor and anti-metastatic activities</t>
+  </si>
+  <si>
+    <t>Novel factor Xa inhibitor, maslinic acid, with antiplatelet aggregation activity</t>
+  </si>
+  <si>
+    <t>Overexpression of OsCM alleviates BLB stress via phytohormonal accumulation and transcriptional modulation of defense-related genes in Oryza sativa</t>
+  </si>
+  <si>
+    <t>Fisetin Suppresses Pulmonary Inflammatory Responses through Heme Oxygenase-1 Mediated Downregulation of Inducible Nitric Oxide Synthase</t>
+  </si>
+  <si>
+    <t>Ferritin Nanocage‐Based Methyltransferase SETD6 for COVID‐19 Therapy</t>
+  </si>
+  <si>
+    <t>Wnt5a and Wnt11 as acute respiratory distress syndrome biomarkers for severe acute respiratory syndrome coronavirus 2 patients</t>
+  </si>
+  <si>
+    <t>Recent progress in therapeutic drug delivery systems for treatment of traumatic CNS injuries</t>
+  </si>
+  <si>
+    <t>The Role of Natural Compounds and their Nanocarriers in the Treatment of CNS Inflammation</t>
+  </si>
+  <si>
+    <t>Inhibitory functions of cardamonin against particulate matter-induced lung injury through TLR2, 4-mTOR-autophagy pathways</t>
+  </si>
+  <si>
+    <t>Phenanthrenes isolated from diocorea batatas Decne peel with anti-platelet aggregation activity via direct factor Xa inhibitory activity</t>
+  </si>
+  <si>
+    <t>Inhibitory effect of oolonghomobisflavan B on osteoclastogenesis by suppressing p38 MAPK activation</t>
+  </si>
+  <si>
+    <t>COVID-19-activated SREBP2 disturbs cholesterol biosynthesis and leads to cytokine storm</t>
+  </si>
+  <si>
+    <t>Novel Herbal Medicine C-KOK Suppresses the Inflammatory Gene iNOS via the Inhibition of p-STAT-1 and NF-κB</t>
+  </si>
+  <si>
+    <t>Identification of suberosin metabolites in human liver microsomes by high‐performance liquid chromatography combined with high‐resolution quadrupole–orbitrap mass spectrometer</t>
+  </si>
+  <si>
     <t>IC Lee, JS Bae</t>
   </si>
   <si>
+    <t>J Kim, S Choo, H Sim, MC Baek, JS Bae</t>
+  </si>
+  <si>
+    <t>Y Kim, JH Kim, T Lee, JS Bae, TC Jeong, ES Lee, S Lee</t>
+  </si>
+  <si>
+    <t>B Khadka, JY Lee, EK Park, KT Kim, JS Bae</t>
+  </si>
+  <si>
+    <t>W Lee, HJ Choi, H Sim, S Choo, GY Song, JS Bae</t>
+  </si>
+  <si>
+    <t>D Hahn, SH Shin, JS Bae</t>
+  </si>
+  <si>
+    <t>YS Choi, H Jang, B Gupta, JH Jeong, Y Ge, CS Yong, JO Kim, JS Bae, ...</t>
+  </si>
+  <si>
+    <t>KM Kim, J Kim, MC Baek, JS Bae</t>
+  </si>
+  <si>
+    <t>R Jan, MA Khan, S Asaf, IJ Lee, JS Bae, KM Kim</t>
+  </si>
+  <si>
+    <t>H Sim, S Choo, J Kim, MC Baek, JS Bae</t>
+  </si>
+  <si>
+    <t>HN Kim, HH Park, W Lim, KS Hong, JH Ahn, DH Na, IS Kim, JG Jang, ...</t>
+  </si>
+  <si>
+    <t>EY Choi, HH Park, H Kim, HN Kim, I Kim, S Jeon, W Kim, JS Bae, W Lee</t>
+  </si>
+  <si>
+    <t>B Khadka, JY Lee, KT Kim, JS Bae</t>
+  </si>
+  <si>
+    <t>B Khadka, JY Lee, DH Park, KT Kim, JS Bae</t>
+  </si>
+  <si>
+    <t>W Lee, D Hahn, H Sim, S Choo, S Lee, T Lee, JS Bae</t>
+  </si>
+  <si>
+    <t>SY Jeong, M Lee, JS Lim, EK Park, MC Baek, JS Kim, D Hahn, JS Bae</t>
+  </si>
+  <si>
+    <t>S Lim, TH Kim, HJ Ihn, J Lim, GY Kim, YH Choi, JS Bae, JC Jung, HI Shin, ...</t>
+  </si>
+  <si>
+    <t>W Lee, JH Ahn, HH Park, HN Kim, H Kim, Y Yoo, H Shin, KS Hong, ...</t>
+  </si>
+  <si>
+    <t>IC Lee, CW Ryu, JS Bae</t>
+  </si>
+  <si>
+    <t>S Paudel, Y Kim, SM Choi, JH Kim, JS Bae, T Lee, S Lee</t>
+  </si>
+  <si>
     <t>Journal of Asian natural products research 23 (2)</t>
   </si>
   <si>
-    <t>Biapenem reduces sepsis mortality via barrier protective pathways against HMGB1-mediated septic responses</t>
-  </si>
-  <si>
-    <t>J Kim, S Choo, H Sim, MC Baek, JS Bae</t>
-  </si>
-  <si>
     <t>Pharmacological Reports</t>
   </si>
   <si>
-    <t>Y Kim, JH Kim, T Lee, JS Bae, TC Jeong, ES Lee, S Lee</t>
-  </si>
-  <si>
     <t>Biopharm Drug Dispos</t>
   </si>
   <si>
-    <t>Impacts of Drug Interactions on Pharmacokinetics and the Brain Transporters: A Recent Review of Natural Compound-Drug Interactions in Brain Disorders</t>
-  </si>
-  <si>
-    <t>B Khadka, JY Lee, EK Park, KT Kim, JS Bae</t>
-  </si>
-  <si>
     <t>International Journal of Molecular Sciences 22 (4)</t>
   </si>
   <si>
-    <t>Barrier protective functions of hederacolchiside-E against HMGB1-mediated septic responses</t>
-  </si>
-  <si>
-    <t>W Lee, HJ Choi, H Sim, S Choo, GY Song, JS Bae</t>
-  </si>
-  <si>
     <t>Pharmacological Research 163</t>
   </si>
   <si>
-    <t>Natural Antioxidant and Anti-Inflammatory Compounds in Foodstuff or Medicinal Herbs Inducing Heme Oxygenase-1 Expression</t>
-  </si>
-  <si>
-    <t>D Hahn, SH Shin, JS Bae</t>
-  </si>
-  <si>
     <t>Antioxidants 9 (12)</t>
   </si>
   <si>
-    <t>Tie2-mediated vascular remodeling by ferritin-based protein C nanoparticles confers antitumor and anti-metastatic activities</t>
-  </si>
-  <si>
-    <t>YS Choi, H Jang, B Gupta, JH Jeong, Y Ge, CS Yong, JO Kim, JS Bae, ...</t>
-  </si>
-  <si>
     <t>Journal of hematology &amp; oncology 13 (1)</t>
   </si>
   <si>
-    <t>Novel factor Xa inhibitor, maslinic acid, with antiplatelet aggregation activity</t>
-  </si>
-  <si>
-    <t>KM Kim, J Kim, MC Baek, JS Bae</t>
-  </si>
-  <si>
     <t>Journal of cellular physiology 235 (12)</t>
   </si>
   <si>
-    <t>Overexpression of OsCM alleviates BLB stress via phytohormonal accumulation and transcriptional modulation of defense-related genes in Oryza sativa</t>
-  </si>
-  <si>
-    <t>R Jan, MA Khan, S Asaf, IJ Lee, JS Bae, KM Kim</t>
-  </si>
-  <si>
     <t>Scientific reports 10 (1)</t>
   </si>
   <si>
-    <t>Fisetin Suppresses Pulmonary Inflammatory Responses through Heme Oxygenase-1 Mediated Downregulation of Inducible Nitric Oxide Synthase</t>
-  </si>
-  <si>
-    <t>H Sim, S Choo, J Kim, MC Baek, JS Bae</t>
-  </si>
-  <si>
     <t>Journal of Medicinal Food 23 (11)</t>
   </si>
   <si>
-    <t>Ferritin Nanocage‐Based Methyltransferase SETD6 for COVID‐19 Therapy</t>
-  </si>
-  <si>
-    <t>HN Kim, HH Park, W Lim, KS Hong, JH Ahn, DH Na, IS Kim, JG Jang, ...</t>
-  </si>
-  <si>
     <t>Advanced Functional Materials 30 (48)</t>
   </si>
   <si>
-    <t>Wnt5a and Wnt11 as acute respiratory distress syndrome biomarkers for severe acute respiratory syndrome coronavirus 2 patients</t>
-  </si>
-  <si>
-    <t>EY Choi, HH Park, H Kim, HN Kim, I Kim, S Jeon, W Kim, JS Bae, W Lee</t>
-  </si>
-  <si>
     <t>European Respiratory Journal 56 (5)</t>
   </si>
   <si>
-    <t>Recent progress in therapeutic drug delivery systems for treatment of traumatic CNS injuries</t>
-  </si>
-  <si>
-    <t>B Khadka, JY Lee, KT Kim, JS Bae</t>
-  </si>
-  <si>
     <t>Future Medicinal Chemistry 12 (19)</t>
   </si>
   <si>
-    <t>The Role of Natural Compounds and their Nanocarriers in the Treatment of CNS Inflammation</t>
-  </si>
-  <si>
-    <t>B Khadka, JY Lee, DH Park, KT Kim, JS Bae</t>
-  </si>
-  <si>
     <t>Biomolecules 10 (10)</t>
   </si>
   <si>
-    <t>Inhibitory functions of cardamonin against particulate matter-induced lung injury through TLR2, 4-mTOR-autophagy pathways</t>
-  </si>
-  <si>
-    <t>W Lee, D Hahn, H Sim, S Choo, S Lee, T Lee, JS Bae</t>
-  </si>
-  <si>
     <t>Fitoterapia 146</t>
   </si>
   <si>
-    <t>Phenanthrenes isolated from diocorea batatas Decne peel with anti-platelet aggregation activity via direct factor Xa inhibitory activity</t>
-  </si>
-  <si>
-    <t>SY Jeong, M Lee, JS Lim, EK Park, MC Baek, JS Kim, D Hahn, JS Bae</t>
-  </si>
-  <si>
     <t>Journal of Functional Foods 73</t>
   </si>
   <si>
-    <t>Inhibitory effect of oolonghomobisflavan B on osteoclastogenesis by suppressing p38 MAPK activation</t>
-  </si>
-  <si>
-    <t>S Lim, TH Kim, HJ Ihn, J Lim, GY Kim, YH Choi, JS Bae, JC Jung, HI Shin, ...</t>
-  </si>
-  <si>
     <t>Bioorganic &amp; Medicinal Chemistry Letters 30 (18)</t>
   </si>
   <si>
-    <t>COVID-19-activated SREBP2 disturbs cholesterol biosynthesis and leads to cytokine storm</t>
-  </si>
-  <si>
-    <t>W Lee, JH Ahn, HH Park, HN Kim, H Kim, Y Yoo, H Shin, KS Hong, ...</t>
-  </si>
-  <si>
     <t>Signal transduction and targeted therapy 5 (1)</t>
   </si>
   <si>
-    <t>Novel Herbal Medicine C-KOK Suppresses the Inflammatory Gene iNOS via the Inhibition of p-STAT-1 and NF-κB</t>
-  </si>
-  <si>
-    <t>IC Lee, CW Ryu, JS Bae</t>
-  </si>
-  <si>
     <t>Biotechnology and Bioprocess Engineering 25 (4)</t>
   </si>
   <si>
-    <t>Identification of suberosin metabolites in human liver microsomes by high‐performance liquid chromatography combined with high‐resolution quadrupole–orbitrap mass spectrometer</t>
-  </si>
-  <si>
-    <t>S Paudel, Y Kim, SM Choi, JH Kim, JS Bae, T Lee, S Lee</t>
-  </si>
-  <si>
     <t>Journal of Mass Spectrometry</t>
   </si>
   <si>
-    <t>Selective inhibitory effects of HYIpro-3-1 on CYP1A2 in human liver microsomes.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2020</t>
   </si>
 </sst>
 </file>
@@ -227,9 +247,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
@@ -274,19 +295,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -306,7 +321,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -348,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,9 +395,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,6 +447,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -590,254 +641,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="77.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="47.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="4"/>
+    <col min="1" max="1" width="70.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="33" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>61</v>
+      <c r="C21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>